<commit_message>
Update GDD & Co
</commit_message>
<xml_diff>
--- a/Feedbacks.xlsx
+++ b/Feedbacks.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\JV\DISTANCE PROJECT\ExpressivePlatformer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\etuln.stockage.univ-lorraine.fr\friche2u\Bureau\Distance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3444083B-CB3A-410E-90F8-A7D56C3D4B3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Feedbacks" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
   <si>
     <t>TO-DO</t>
   </si>
@@ -40,9 +39,6 @@
   </si>
   <si>
     <t>Feedbacks</t>
-  </si>
-  <si>
-    <t>Animations</t>
   </si>
   <si>
     <t>Sons</t>
@@ -119,11 +115,164 @@
   <si>
     <t>Liste des sons</t>
   </si>
+  <si>
+    <t>Dash</t>
+  </si>
+  <si>
+    <t>Saut Mural</t>
+  </si>
+  <si>
+    <t>Saut Double</t>
+  </si>
+  <si>
+    <t>Dash Qui Pousse</t>
+  </si>
+  <si>
+    <t>Dash (???)</t>
+  </si>
+  <si>
+    <t>déclenché par joueur</t>
+  </si>
+  <si>
+    <t>Contact avec PNJ</t>
+  </si>
+  <si>
+    <t>Tomber Trou</t>
+  </si>
+  <si>
+    <t>Dash qui pousse</t>
+  </si>
+  <si>
+    <t>Contact avec PnJ</t>
+  </si>
+  <si>
+    <t>Mort du joueur</t>
+  </si>
+  <si>
+    <t>Contact avec Outil de communication</t>
+  </si>
+  <si>
+    <t>Le personnage se déplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Animations ou FX graphique</t>
+  </si>
+  <si>
+    <t>Tomber au sol</t>
+  </si>
+  <si>
+    <t>FX d'onde de choc (petit)</t>
+  </si>
+  <si>
+    <t>FX onde de choc (moyen)</t>
+  </si>
+  <si>
+    <t>FX onde de choc (grand)</t>
+  </si>
+  <si>
+    <t>Pareil avec FX onde de choc derrière perso</t>
+  </si>
+  <si>
+    <t>FX yeux qui s'illuminent selon couleur PNJ</t>
+  </si>
+  <si>
+    <t>FX onde de choc (petit)</t>
+  </si>
+  <si>
+    <t>FX traits + particule couleur perso + FX cape qui bouge + FrzFm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personnage ferme yeux, reflet lumière sur tête </t>
+  </si>
+  <si>
+    <t>Tableau/Niveau</t>
+  </si>
+  <si>
+    <t>Effet de brume</t>
+  </si>
+  <si>
+    <t>Changement d'écran de tableau</t>
+  </si>
+  <si>
+    <t>Changement d'écran de niveau</t>
+  </si>
+  <si>
+    <t>PNJs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apparition </t>
+  </si>
+  <si>
+    <t>Déplacement</t>
+  </si>
+  <si>
+    <t>Bruit de flamme + reverb</t>
+  </si>
+  <si>
+    <t>Image rémanante derrière le spectre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoom Sur joueur </t>
+  </si>
+  <si>
+    <t>Bruit de pas sur bois</t>
+  </si>
+  <si>
+    <t>souffle</t>
+  </si>
+  <si>
+    <t>Souffle + sub bass</t>
+  </si>
+  <si>
+    <t>animation rapide du sprite qui devient transparent puis full</t>
+  </si>
+  <si>
+    <t>un "tic" bref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halo autour du joueur </t>
+  </si>
+  <si>
+    <t>Effet de brume plus long, fade sur écran noir</t>
+  </si>
+  <si>
+    <t>effet distortion sur écran</t>
+  </si>
+  <si>
+    <t>bruit aigu, sharp</t>
+  </si>
+  <si>
+    <t>Collisions</t>
+  </si>
+  <si>
+    <t>Dash qui pousse VS tronc qui tombe</t>
+  </si>
+  <si>
+    <t>ScrShk puis arbre qui rotate de vertical à horizontal (lentement)</t>
+  </si>
+  <si>
+    <t>Chute objet lourd</t>
+  </si>
+  <si>
+    <t>Dash qui pousse VS objet inaltérable</t>
+  </si>
+  <si>
+    <t>Petit rebond du personnage</t>
+  </si>
+  <si>
+    <t>pareil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "fail"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12">
     <font>
       <sz val="10"/>
@@ -609,10 +758,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -761,6 +906,10 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1186,23 +1335,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="11" customWidth="1"/>
     <col min="2" max="2" width="44.5703125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="74.28515625" style="11" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="11" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" style="11" customWidth="1"/>
     <col min="7" max="7" width="11" style="11" customWidth="1"/>
     <col min="8" max="8" width="15.140625" style="11" customWidth="1"/>
@@ -1273,23 +1422,23 @@
         <v>4</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="F3" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="74"/>
+      <c r="H3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19" t="s">
+      <c r="I3" s="18" t="s">
         <v>9</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>10</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="10"/>
@@ -1310,25 +1459,29 @@
       <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="21" t="s">
-        <v>15</v>
+      <c r="A4" s="19" t="s">
+        <v>14</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>20</v>
+      <c r="B4" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27" t="s">
+      <c r="C4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="27" t="s">
         <v>11</v>
-      </c>
-      <c r="J4" s="29" t="s">
-        <v>12</v>
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
@@ -1348,23 +1501,27 @@
       <c r="Z4" s="10"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31" t="s">
-        <v>21</v>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29" t="s">
+        <v>20</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36" t="s">
+      <c r="C5" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="27" t="s">
         <v>13</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>14</v>
       </c>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
@@ -1384,19 +1541,25 @@
       <c r="Z5" s="10"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="30"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="28" t="s">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="27" t="s">
         <v>16</v>
-      </c>
-      <c r="J6" s="29" t="s">
-        <v>17</v>
       </c>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
@@ -1416,19 +1579,25 @@
       <c r="Z6" s="10"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="30"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="28" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="27" t="s">
         <v>18</v>
-      </c>
-      <c r="J7" s="29" t="s">
-        <v>19</v>
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
@@ -1448,15 +1617,21 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="30"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="38"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="36"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -1475,15 +1650,23 @@
       <c r="Z8" s="10"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="30"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="39"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="34"/>
+      <c r="I9" s="37"/>
       <c r="J9" s="12"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
@@ -1503,15 +1686,21 @@
       <c r="Z9" s="10"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="30"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="40"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="12"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -1531,15 +1720,21 @@
       <c r="Z10" s="10"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="30"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="41"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="12"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
@@ -1559,14 +1754,20 @@
       <c r="Z11" s="10"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="30"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="36"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="34"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="10"/>
@@ -1587,14 +1788,22 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="30"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="36"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="28"/>
+      <c r="H13" s="34"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="10"/>
@@ -1615,14 +1824,22 @@
       <c r="Z13" s="10"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="30"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="36"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="34"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="10"/>
@@ -1643,14 +1860,14 @@
       <c r="Z14" s="10"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="30"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="36"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="10"/>
@@ -1671,14 +1888,14 @@
       <c r="Z15" s="10"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="30"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="36"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="34"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="10"/>
@@ -1699,14 +1916,14 @@
       <c r="Z16" s="10"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A17" s="30"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="36"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="34"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="10"/>
@@ -1727,14 +1944,22 @@
       <c r="Z17" s="10"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A18" s="30"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="36"/>
+      <c r="A18" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="34"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="K18" s="10"/>
@@ -1755,14 +1980,20 @@
       <c r="Z18" s="10"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A19" s="30"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="36"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="34"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="10"/>
@@ -1783,14 +2014,14 @@
       <c r="Z19" s="10"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A20" s="30"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="36"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="34"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="10"/>
@@ -1811,14 +2042,22 @@
       <c r="Z20" s="10"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A21" s="30"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="36"/>
+      <c r="A21" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="34"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="10"/>
@@ -1839,14 +2078,18 @@
       <c r="Z21" s="10"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A22" s="30"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="36"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="34"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="10"/>
@@ -1867,14 +2110,14 @@
       <c r="Z22" s="10"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A23" s="30"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="36"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="34"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="10"/>
@@ -1895,14 +2138,22 @@
       <c r="Z23" s="10"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A24" s="30"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="36"/>
+      <c r="A24" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="34"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="10"/>
@@ -1923,14 +2174,20 @@
       <c r="Z24" s="10"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A25" s="30"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="36"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="34"/>
       <c r="I25" s="10"/>
       <c r="J25" s="12"/>
       <c r="K25" s="10"/>
@@ -1951,14 +2208,14 @@
       <c r="Z25" s="10"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A26" s="30"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="36"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="34"/>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
@@ -1979,14 +2236,14 @@
       <c r="Z26" s="10"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A27" s="42"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="44"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="42"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
@@ -2043,7 +2300,7 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="45"/>
+      <c r="I29" s="43"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
@@ -28949,7 +29206,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1">
           <x14:formula1>
             <xm:f>'()'!$A$1:$A$4</xm:f>
           </x14:formula1>
@@ -28962,11 +29219,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FF4F28-5B93-41A6-927B-922DB95A95B0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -28991,8 +29248,8 @@
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="2:11" ht="21">
-      <c r="B2" s="73" t="s">
-        <v>30</v>
+      <c r="B2" s="71" t="s">
+        <v>29</v>
       </c>
       <c r="G2" s="6"/>
       <c r="I2" s="7"/>
@@ -29004,319 +29261,347 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="D4" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="E4" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="F4" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="G4" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="57" t="s">
-        <v>9</v>
+      <c r="H4" s="55" t="s">
+        <v>8</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="2:11" ht="15">
-      <c r="B5" s="46" t="s">
-        <v>15</v>
+      <c r="B5" s="44" t="s">
+        <v>14</v>
       </c>
-      <c r="C5" s="59" t="s">
-        <v>20</v>
+      <c r="C5" s="57" t="s">
+        <v>19</v>
       </c>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="64" t="s">
-        <v>28</v>
+      <c r="D5" s="59" t="s">
+        <v>35</v>
       </c>
-      <c r="G5" s="69" t="s">
+      <c r="E5" s="59"/>
+      <c r="F5" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="66" t="s">
-        <v>29</v>
+      <c r="G5" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="64" t="s">
+        <v>28</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="9"/>
     </row>
     <row r="6" spans="2:11" ht="15">
-      <c r="B6" s="47"/>
-      <c r="C6" s="60" t="s">
-        <v>21</v>
+      <c r="B6" s="45"/>
+      <c r="C6" s="58" t="s">
+        <v>20</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="65" t="s">
+      <c r="D6" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="60"/>
+      <c r="F6" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="68"/>
+      <c r="H6" s="65" t="s">
         <v>28</v>
-      </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="67" t="s">
-        <v>29</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="2:11" ht="15">
-      <c r="B7" s="48"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="49"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="47"/>
     </row>
     <row r="8" spans="2:11" ht="15">
-      <c r="B8" s="48"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="49"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="47"/>
     </row>
     <row r="9" spans="2:11" ht="15">
-      <c r="B9" s="48"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="49"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="47"/>
     </row>
     <row r="10" spans="2:11" ht="15">
-      <c r="B10" s="48"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="49"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="47"/>
     </row>
     <row r="11" spans="2:11" ht="15">
-      <c r="B11" s="48"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="49"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="47"/>
     </row>
     <row r="12" spans="2:11" ht="15">
-      <c r="B12" s="48"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="49"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="61"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="2:11" ht="15">
-      <c r="B13" s="48"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="49"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="61"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="47"/>
     </row>
     <row r="14" spans="2:11" ht="15">
-      <c r="B14" s="50"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="49"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="47"/>
     </row>
     <row r="15" spans="2:11" ht="15">
-      <c r="B15" s="48"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="49"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="47"/>
     </row>
     <row r="16" spans="2:11" ht="15">
-      <c r="B16" s="48"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="49"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="47"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="48"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="49"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="47"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="48"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="49"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="47"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="51"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="47"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="51"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="49"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="47"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="51"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="49"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="47"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="51"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="49"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="47"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="51"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="49"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="47"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="51"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="49"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="47"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="51"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="49"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="47"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="51"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="47"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="51"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="49"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="47"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="51"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="49"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="47"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="51"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="49"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="47"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="51"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="49"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="47"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="52"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="72"/>
-      <c r="H31" s="53"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="51"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
     </row>
@@ -34130,21 +34415,21 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{6593282D-BD3C-42BC-97A5-F5D9493C0105}">
+        <x14:dataValidation type="list" allowBlank="1">
           <x14:formula1>
-            <xm:f>[Sons.xlsx]Feuil2!#REF!</xm:f>
+            <xm:f>'G:\Documents\JV\DISTANCE PROJECT\ExpressivePlatformer\[Sons.xlsx]Feuil2'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G5:G6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{DE878B5F-2884-4E72-8C4D-42488AFB8A25}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[Sons.xlsx]Feuil2!#REF!</xm:f>
+            <xm:f>'G:\Documents\JV\DISTANCE PROJECT\ExpressivePlatformer\[Sons.xlsx]Feuil2'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>F5:F6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{0E8F8875-CADF-46BC-946A-6A213B344E1F}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[Sons.xlsx]Feuil2!#REF!</xm:f>
+            <xm:f>'G:\Documents\JV\DISTANCE PROJECT\ExpressivePlatformer\[Sons.xlsx]Feuil2'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>H5:H6</xm:sqref>
         </x14:dataValidation>
@@ -34155,7 +34440,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>

<commit_message>
Ajouts et corrections Feedbacks
</commit_message>
<xml_diff>
--- a/Feedbacks.xlsx
+++ b/Feedbacks.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\etuln.stockage.univ-lorraine.fr\friche2u\Bureau\Distance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\JV\DISTANCE PROJECT\ExpressivePlatformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9885D474-BF24-4F08-B4DC-6ABBC713CB0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedbacks" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="83">
   <si>
     <t>TO-DO</t>
   </si>
@@ -152,37 +153,16 @@
     <t>Contact avec Outil de communication</t>
   </si>
   <si>
-    <t>Le personnage se déplace</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Animations ou FX graphique</t>
   </si>
   <si>
     <t>Tomber au sol</t>
   </si>
   <si>
-    <t>FX d'onde de choc (petit)</t>
-  </si>
-  <si>
-    <t>FX onde de choc (moyen)</t>
-  </si>
-  <si>
-    <t>FX onde de choc (grand)</t>
-  </si>
-  <si>
-    <t>Pareil avec FX onde de choc derrière perso</t>
-  </si>
-  <si>
     <t>FX yeux qui s'illuminent selon couleur PNJ</t>
   </si>
   <si>
     <t>FX onde de choc (petit)</t>
-  </si>
-  <si>
-    <t>FX traits + particule couleur perso + FX cape qui bouge + FrzFm</t>
   </si>
   <si>
     <t xml:space="preserve">Personnage ferme yeux, reflet lumière sur tête </t>
@@ -251,9 +231,6 @@
     <t>Dash qui pousse VS tronc qui tombe</t>
   </si>
   <si>
-    <t>ScrShk puis arbre qui rotate de vertical à horizontal (lentement)</t>
-  </si>
-  <si>
     <t>Chute objet lourd</t>
   </si>
   <si>
@@ -268,11 +245,41 @@
   <si>
     <t xml:space="preserve"> "fail"</t>
   </si>
+  <si>
+    <t>FX traits + particule couleur perso + animation cape qui bouge</t>
+  </si>
+  <si>
+    <t>FX traits + particule couleur perso + animation cape qui bouge + onde de choc derrière perso</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Arbre qui rotate de vertical à horizontal (lentement) + particules quand touche le sol</t>
+  </si>
+  <si>
+    <t>oo</t>
+  </si>
+  <si>
+    <t>ooo</t>
+  </si>
+  <si>
+    <t>Animation de marche</t>
+  </si>
+  <si>
+    <t>Anim saut + FX d'onde de choc (petit)</t>
+  </si>
+  <si>
+    <t>Anim saut + FX onde de choc (moyen)</t>
+  </si>
+  <si>
+    <t>Anim saut + FX onde de choc (grand)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12">
     <font>
       <sz val="10"/>
@@ -343,7 +350,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,8 +429,26 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -504,35 +529,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -567,26 +563,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -710,11 +686,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -764,25 +755,7 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -791,28 +764,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -825,96 +777,117 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="88">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1003,12 +976,892 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCCC"/>
       <color rgb="FFCCCCFF"/>
-      <color rgb="FFFFCCCC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1335,21 +2188,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="11" customWidth="1"/>
     <col min="2" max="2" width="44.5703125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="74.28515625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="78.28515625" style="11" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" style="11" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" style="11" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" style="11" customWidth="1"/>
@@ -1422,7 +2275,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>5</v>
@@ -1430,10 +2283,10 @@
       <c r="E3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="73" t="s">
+      <c r="F3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="74"/>
+      <c r="G3" s="59"/>
       <c r="H3" s="17" t="s">
         <v>8</v>
       </c>
@@ -1462,25 +2315,31 @@
       <c r="A4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>42</v>
+      <c r="C4" s="60" t="s">
+        <v>79</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>64</v>
+      <c r="D4" s="61" t="s">
+        <v>57</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25" t="s">
+      <c r="E4" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="21" t="s">
         <v>11</v>
       </c>
       <c r="K4" s="10"/>
@@ -1501,26 +2360,32 @@
       <c r="Z4" s="10"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>46</v>
+      <c r="C5" s="60" t="s">
+        <v>80</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34" t="s">
+      <c r="E5" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="21" t="s">
         <v>13</v>
       </c>
       <c r="K5" s="10"/>
@@ -1541,24 +2406,32 @@
       <c r="Z5" s="10"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="28" t="s">
-        <v>47</v>
+      <c r="C6" s="64" t="s">
+        <v>81</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="26" t="s">
+      <c r="E6" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="21" t="s">
         <v>16</v>
       </c>
       <c r="K6" s="10"/>
@@ -1579,24 +2452,32 @@
       <c r="Z6" s="10"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>48</v>
+      <c r="C7" s="64" t="s">
+        <v>82</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="26" t="s">
+      <c r="E7" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="21" t="s">
         <v>18</v>
       </c>
       <c r="K7" s="10"/>
@@ -1617,21 +2498,29 @@
       <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>52</v>
+      <c r="C8" s="64" t="s">
+        <v>73</v>
       </c>
-      <c r="D8" s="28" t="s">
-        <v>72</v>
+      <c r="D8" s="65" t="s">
+        <v>65</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="36"/>
+      <c r="E8" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="23"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -1650,23 +2539,29 @@
       <c r="Z8" s="10"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="28" t="s">
-        <v>49</v>
+      <c r="C9" s="64" t="s">
+        <v>74</v>
       </c>
-      <c r="D9" s="28" t="s">
-        <v>79</v>
+      <c r="D9" s="65" t="s">
+        <v>71</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28" t="s">
-        <v>12</v>
+      <c r="E9" s="62" t="s">
+        <v>15</v>
       </c>
-      <c r="H9" s="34"/>
-      <c r="I9" s="37"/>
+      <c r="F9" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="24"/>
       <c r="J9" s="12"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
@@ -1686,21 +2581,29 @@
       <c r="Z9" s="10"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="28" t="s">
-        <v>43</v>
+      <c r="C10" s="64" t="s">
+        <v>75</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="38"/>
+      <c r="G10" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="25"/>
       <c r="J10" s="12"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -1720,21 +2623,29 @@
       <c r="Z10" s="10"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="28" t="s">
-        <v>50</v>
+      <c r="C11" s="64" t="s">
+        <v>44</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28" t="s">
-        <v>63</v>
+      <c r="D11" s="65" t="s">
+        <v>75</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="39"/>
+      <c r="E11" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="26"/>
       <c r="J11" s="12"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
@@ -1754,20 +2665,28 @@
       <c r="Z11" s="10"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>53</v>
+      <c r="C12" s="64" t="s">
+        <v>46</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28" t="s">
-        <v>63</v>
+      <c r="D12" s="65" t="s">
+        <v>75</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="34"/>
+      <c r="E12" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="68" t="s">
+        <v>0</v>
+      </c>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="10"/>
@@ -1788,22 +2707,28 @@
       <c r="Z12" s="10"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>69</v>
+      <c r="C13" s="64" t="s">
+        <v>62</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28" t="s">
-        <v>71</v>
+      <c r="D13" s="65" t="s">
+        <v>75</v>
       </c>
-      <c r="F13" s="28" t="s">
-        <v>12</v>
+      <c r="E13" s="62" t="s">
+        <v>64</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="34"/>
+      <c r="F13" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="68" t="s">
+        <v>0</v>
+      </c>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="10"/>
@@ -1824,22 +2749,28 @@
       <c r="Z13" s="10"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="67" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="28" t="s">
-        <v>51</v>
+      <c r="D14" s="65" t="s">
+        <v>61</v>
       </c>
-      <c r="D14" s="28" t="s">
-        <v>68</v>
+      <c r="E14" s="62" t="s">
+        <v>10</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28" t="s">
+      <c r="F14" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="34"/>
+      <c r="H14" s="68" t="s">
+        <v>0</v>
+      </c>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="10"/>
@@ -1860,14 +2791,14 @@
       <c r="Z14" s="10"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="28"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="34"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="68"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="10"/>
@@ -1888,14 +2819,14 @@
       <c r="Z15" s="10"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="28"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="34"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="68"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="10"/>
@@ -1916,14 +2847,14 @@
       <c r="Z16" s="10"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A17" s="28"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="34"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="68"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="10"/>
@@ -1944,22 +2875,30 @@
       <c r="Z17" s="10"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A18" s="28" t="s">
-        <v>54</v>
+      <c r="A18" s="22" t="s">
+        <v>47</v>
       </c>
-      <c r="B18" s="29" t="s">
-        <v>56</v>
+      <c r="B18" s="67" t="s">
+        <v>49</v>
       </c>
-      <c r="C18" s="28" t="s">
-        <v>55</v>
+      <c r="C18" s="64" t="s">
+        <v>48</v>
       </c>
-      <c r="D18" s="28" t="s">
-        <v>65</v>
+      <c r="D18" s="65" t="s">
+        <v>58</v>
       </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="34"/>
+      <c r="E18" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="68" t="s">
+        <v>1</v>
+      </c>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="K18" s="10"/>
@@ -1980,20 +2919,28 @@
       <c r="Z18" s="10"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A19" s="28"/>
-      <c r="B19" s="29" t="s">
-        <v>57</v>
+      <c r="A19" s="22"/>
+      <c r="B19" s="67" t="s">
+        <v>50</v>
       </c>
-      <c r="C19" s="28" t="s">
-        <v>70</v>
+      <c r="C19" s="64" t="s">
+        <v>63</v>
       </c>
-      <c r="D19" s="28" t="s">
-        <v>66</v>
+      <c r="D19" s="65" t="s">
+        <v>59</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="34"/>
+      <c r="E19" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="68" t="s">
+        <v>1</v>
+      </c>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="10"/>
@@ -2014,14 +2961,14 @@
       <c r="Z19" s="10"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A20" s="28"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="34"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="68"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="10"/>
@@ -2042,22 +2989,30 @@
       <c r="Z20" s="10"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A21" s="28" t="s">
-        <v>58</v>
+      <c r="A21" s="22" t="s">
+        <v>51</v>
       </c>
-      <c r="B21" s="35" t="s">
-        <v>59</v>
+      <c r="B21" s="67" t="s">
+        <v>52</v>
       </c>
-      <c r="C21" s="28" t="s">
-        <v>67</v>
+      <c r="C21" s="64" t="s">
+        <v>60</v>
       </c>
-      <c r="D21" s="28" t="s">
-        <v>61</v>
+      <c r="D21" s="65" t="s">
+        <v>54</v>
       </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="34"/>
+      <c r="E21" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="68" t="s">
+        <v>0</v>
+      </c>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="10"/>
@@ -2078,18 +3033,26 @@
       <c r="Z21" s="10"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A22" s="28"/>
-      <c r="B22" s="35" t="s">
-        <v>60</v>
+      <c r="A22" s="22"/>
+      <c r="B22" s="67" t="s">
+        <v>53</v>
       </c>
-      <c r="C22" s="28" t="s">
-        <v>62</v>
+      <c r="C22" s="64" t="s">
+        <v>55</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="34"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="68" t="s">
+        <v>0</v>
+      </c>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="10"/>
@@ -2110,14 +3073,14 @@
       <c r="Z22" s="10"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A23" s="28"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="34"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="68"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="10"/>
@@ -2138,22 +3101,30 @@
       <c r="Z23" s="10"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A24" s="28" t="s">
-        <v>73</v>
+      <c r="A24" s="22" t="s">
+        <v>66</v>
       </c>
-      <c r="B24" s="35" t="s">
-        <v>74</v>
+      <c r="B24" s="67" t="s">
+        <v>67</v>
       </c>
-      <c r="C24" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="28" t="s">
+      <c r="C24" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="34"/>
+      <c r="D24" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="68" t="s">
+        <v>0</v>
+      </c>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="10"/>
@@ -2174,20 +3145,28 @@
       <c r="Z24" s="10"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A25" s="28"/>
-      <c r="B25" s="35" t="s">
-        <v>77</v>
+      <c r="A25" s="22"/>
+      <c r="B25" s="67" t="s">
+        <v>69</v>
       </c>
-      <c r="C25" s="28" t="s">
-        <v>78</v>
+      <c r="C25" s="64" t="s">
+        <v>70</v>
       </c>
-      <c r="D25" s="28" t="s">
-        <v>80</v>
+      <c r="D25" s="65" t="s">
+        <v>72</v>
       </c>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="34"/>
+      <c r="E25" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="68" t="s">
+        <v>0</v>
+      </c>
       <c r="I25" s="10"/>
       <c r="J25" s="12"/>
       <c r="K25" s="10"/>
@@ -2208,14 +3187,14 @@
       <c r="Z25" s="10"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A26" s="28"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="34"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="68"/>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
@@ -2236,14 +3215,14 @@
       <c r="Z26" s="10"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A27" s="40"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="42"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="68"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
@@ -2300,7 +3279,7 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="43"/>
+      <c r="I29" s="28"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
@@ -29182,23 +30161,423 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:H5">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="87" priority="81" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H5">
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="86" priority="82" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H5">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="85" priority="83" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H5">
+    <cfRule type="containsText" dxfId="84" priority="84" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="containsText" dxfId="83" priority="77" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H6))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="containsText" dxfId="82" priority="78" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H6))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="containsText" dxfId="81" priority="79" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H6))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="containsText" dxfId="80" priority="80" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H6))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="containsText" dxfId="79" priority="73" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H7))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="containsText" dxfId="78" priority="74" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H7))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="containsText" dxfId="77" priority="75" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H7))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="containsText" dxfId="76" priority="76" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H7))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="containsText" dxfId="75" priority="69" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H8))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="containsText" dxfId="74" priority="70" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H8))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="containsText" dxfId="73" priority="71" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H8))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="containsText" dxfId="72" priority="72" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H8))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="containsText" dxfId="71" priority="65" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="containsText" dxfId="70" priority="66" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="containsText" dxfId="69" priority="67" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="containsText" dxfId="68" priority="68" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="containsText" dxfId="67" priority="61" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="containsText" dxfId="66" priority="62" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="containsText" dxfId="65" priority="63" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="containsText" dxfId="64" priority="64" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="containsText" dxfId="63" priority="57" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H11))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="containsText" dxfId="62" priority="58" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H11))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="containsText" dxfId="61" priority="59" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H11))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="containsText" dxfId="60" priority="60" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H11))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="containsText" dxfId="59" priority="53" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="containsText" dxfId="58" priority="54" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="containsText" dxfId="57" priority="55" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="containsText" dxfId="56" priority="56" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="containsText" dxfId="55" priority="49" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="containsText" dxfId="54" priority="50" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="containsText" dxfId="53" priority="51" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="containsText" dxfId="52" priority="52" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="containsText" dxfId="51" priority="45" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="containsText" dxfId="50" priority="46" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="containsText" dxfId="47" priority="41" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="containsText" dxfId="46" priority="42" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="containsText" dxfId="45" priority="43" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="containsText" dxfId="44" priority="44" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="containsText" dxfId="43" priority="37" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="containsText" dxfId="42" priority="38" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="containsText" dxfId="41" priority="39" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="containsText" dxfId="40" priority="40" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="containsText" dxfId="39" priority="33" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H17))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="containsText" dxfId="38" priority="34" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H17))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H17))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H17))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="containsText" dxfId="35" priority="29" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="containsText" dxfId="34" priority="30" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="containsText" dxfId="28" priority="28" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H25))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H25))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H25))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
     <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TO REWORK">
-      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H4))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H25))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29206,11 +30585,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'()'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H4:H5</xm:sqref>
+          <xm:sqref>H4:H25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -29219,11 +30598,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:K988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -29248,7 +30627,7 @@
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="2:11" ht="21">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="56" t="s">
         <v>29</v>
       </c>
       <c r="G2" s="6"/>
@@ -29261,25 +30640,25 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="55" t="s">
+      <c r="H4" s="40" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="8"/>
@@ -29287,23 +30666,23 @@
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="2:11" ht="15">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="62" t="s">
+      <c r="E5" s="44"/>
+      <c r="F5" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="64" t="s">
+      <c r="H5" s="49" t="s">
         <v>28</v>
       </c>
       <c r="I5" s="7"/>
@@ -29311,19 +30690,19 @@
       <c r="K5" s="9"/>
     </row>
     <row r="6" spans="2:11" ht="15">
-      <c r="B6" s="45"/>
-      <c r="C6" s="58" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="63" t="s">
+      <c r="E6" s="45"/>
+      <c r="F6" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="68"/>
-      <c r="H6" s="65" t="s">
+      <c r="G6" s="53"/>
+      <c r="H6" s="50" t="s">
         <v>28</v>
       </c>
       <c r="I6" s="7"/>
@@ -29331,277 +30710,277 @@
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="2:11" ht="15">
-      <c r="B7" s="46"/>
-      <c r="C7" s="52" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="61" t="s">
+      <c r="D7" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="47"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="2:11" ht="15">
-      <c r="B8" s="46"/>
-      <c r="C8" s="52" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="47"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="2:11" ht="15">
-      <c r="B9" s="46"/>
-      <c r="C9" s="52" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="47"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="2:11" ht="15">
-      <c r="B10" s="46"/>
-      <c r="C10" s="52" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="47"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="32"/>
     </row>
     <row r="11" spans="2:11" ht="15">
-      <c r="B11" s="46"/>
-      <c r="C11" s="52" t="s">
+      <c r="B11" s="31"/>
+      <c r="C11" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="61" t="s">
+      <c r="D11" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="47"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="32"/>
     </row>
     <row r="12" spans="2:11" ht="15">
-      <c r="B12" s="46"/>
-      <c r="C12" s="52" t="s">
+      <c r="B12" s="31"/>
+      <c r="C12" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="61"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="47"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="32"/>
     </row>
     <row r="13" spans="2:11" ht="15">
-      <c r="B13" s="46"/>
-      <c r="C13" s="52" t="s">
+      <c r="B13" s="31"/>
+      <c r="C13" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="61"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="47"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="2:11" ht="15">
-      <c r="B14" s="48"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="47"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="2:11" ht="15">
-      <c r="B15" s="46"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="47"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="2:11" ht="15">
-      <c r="B16" s="46"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="47"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="32"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B17" s="46"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="47"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B18" s="46"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="47"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="32"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B19" s="49"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="47"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="32"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B20" s="49"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="47"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="32"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B21" s="49"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="47"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="32"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B22" s="49"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="47"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="32"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B23" s="49"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="47"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="32"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B24" s="49"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="47"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="32"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B25" s="49"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="47"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="32"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B26" s="49"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="47"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="32"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B27" s="49"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="47"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="32"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
     </row>
     <row r="28" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B28" s="49"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="47"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="32"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B29" s="49"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="47"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="32"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" customHeight="1">
-      <c r="B30" s="49"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="47"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="32"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B31" s="50"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="51"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="36"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
     </row>
@@ -34414,24 +35793,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'G:\Documents\JV\DISTANCE PROJECT\ExpressivePlatformer\[Sons.xlsx]Feuil2'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G5:G6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'G:\Documents\JV\DISTANCE PROJECT\ExpressivePlatformer\[Sons.xlsx]Feuil2'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>F5:F6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'G:\Documents\JV\DISTANCE PROJECT\ExpressivePlatformer\[Sons.xlsx]Feuil2'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>H5:H6</xm:sqref>
+          <xm:sqref>F5:F6 H5:H6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -34440,7 +35813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>

<commit_message>
Fx sorties + mort + dash
</commit_message>
<xml_diff>
--- a/Feedbacks.xlsx
+++ b/Feedbacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\JV\DISTANCE PROJECT\ExpressivePlatformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB36E4B1-214C-46BF-97E9-A8D9D0CA71B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A20056-C5A9-4518-A67F-4D48BB052C39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="100">
   <si>
     <t>TO-DO</t>
   </si>
@@ -316,6 +316,18 @@
   <si>
     <t>Validate</t>
   </si>
+  <si>
+    <t>Idle Spectre</t>
+  </si>
+  <si>
+    <t>Spectre</t>
+  </si>
+  <si>
+    <t>Idle Perso</t>
+  </si>
+  <si>
+    <t>Animation idle</t>
+  </si>
 </sst>
 </file>
 
@@ -385,7 +397,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -467,6 +479,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor rgb="FFD9E2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor rgb="FFE2EFD9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
@@ -744,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -920,9 +968,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -938,10 +983,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2132,7 +2216,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2220,10 +2304,10 @@
       <c r="E3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="73" t="s">
+      <c r="F3" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="74"/>
+      <c r="G3" s="83"/>
       <c r="H3" s="41" t="s">
         <v>16</v>
       </c>
@@ -2271,7 +2355,7 @@
         <v>33</v>
       </c>
       <c r="H4" s="49" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4" s="50" t="s">
         <v>33</v>
@@ -2317,7 +2401,7 @@
         <v>33</v>
       </c>
       <c r="H5" s="49" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="50" t="s">
         <v>37</v>
@@ -2363,7 +2447,7 @@
         <v>33</v>
       </c>
       <c r="H6" s="49" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="50" t="s">
         <v>41</v>
@@ -2409,7 +2493,7 @@
         <v>33</v>
       </c>
       <c r="H7" s="49" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="50" t="s">
         <v>44</v>
@@ -2455,7 +2539,7 @@
         <v>37</v>
       </c>
       <c r="H8" s="49" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="57"/>
       <c r="J8" s="1"/>
@@ -2497,7 +2581,7 @@
         <v>51</v>
       </c>
       <c r="H9" s="49" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="58"/>
       <c r="J9" s="9"/>
@@ -2607,24 +2691,22 @@
       <c r="B12" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="48" t="s">
+      <c r="F12" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="48" t="s">
+      <c r="G12" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="49" t="s">
-        <v>0</v>
-      </c>
+      <c r="H12" s="76"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="8"/>
@@ -2665,7 +2747,7 @@
         <v>33</v>
       </c>
       <c r="H13" s="49" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -2707,7 +2789,7 @@
         <v>37</v>
       </c>
       <c r="H14" s="49" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -2730,26 +2812,26 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="51"/>
-      <c r="B15" s="59" t="s">
-        <v>69</v>
+      <c r="B15" s="77" t="s">
+        <v>98</v>
       </c>
-      <c r="C15" s="60" t="s">
-        <v>70</v>
+      <c r="C15" s="78" t="s">
+        <v>99</v>
       </c>
-      <c r="D15" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="61" t="s">
+      <c r="D15" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="62" t="s">
+      <c r="E15" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="62" t="s">
+      <c r="F15" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="79" t="s">
         <v>33</v>
       </c>
       <c r="H15" s="66" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -2771,14 +2853,30 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="51"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="49"/>
+      <c r="A16" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="49" t="s">
+        <v>1</v>
+      </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="8"/>
@@ -2800,13 +2898,27 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="51"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49"/>
+      <c r="B17" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="66" t="s">
+        <v>0</v>
+      </c>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="8"/>
@@ -2986,27 +3098,25 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="51"/>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="47" t="s">
+      <c r="E22" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="48" t="s">
+      <c r="F22" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="48" t="s">
+      <c r="G22" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="H22" s="49" t="s">
-        <v>0</v>
-      </c>
+      <c r="H22" s="76"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="8"/>
@@ -3169,7 +3279,7 @@
       <c r="Z26" s="8"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="68" t="s">
+      <c r="A27" s="67" t="s">
         <v>93</v>
       </c>
       <c r="B27" s="59" t="s">
@@ -3211,9 +3321,9 @@
       <c r="B28" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="69"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="70"/>
       <c r="F28" s="62" t="s">
         <v>33</v>
       </c>
@@ -3251,7 +3361,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
-      <c r="I29" s="72"/>
+      <c r="I29" s="71"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
@@ -30463,423 +30573,423 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:H5">
-    <cfRule type="containsText" dxfId="87" priority="1" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="87" priority="5" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H5">
-    <cfRule type="containsText" dxfId="86" priority="2" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="86" priority="6" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H5">
-    <cfRule type="containsText" dxfId="85" priority="3" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="85" priority="7" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H5">
-    <cfRule type="containsText" dxfId="84" priority="4" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="84" priority="8" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="83" priority="5" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="83" priority="9" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="82" priority="6" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="82" priority="10" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="81" priority="7" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="81" priority="11" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="80" priority="8" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="80" priority="12" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="79" priority="9" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="79" priority="13" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H7))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="78" priority="10" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="78" priority="14" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H7))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="77" priority="11" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="77" priority="15" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H7))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="76" priority="12" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="76" priority="16" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H7))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="75" priority="13" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="75" priority="17" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H8))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="74" priority="14" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="74" priority="18" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H8))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="73" priority="15" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="73" priority="19" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H8))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="72" priority="16" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="72" priority="20" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H8))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="71" priority="17" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="71" priority="21" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="70" priority="18" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="70" priority="22" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="69" priority="19" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="69" priority="23" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="containsText" dxfId="68" priority="20" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="68" priority="24" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="67" priority="21" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="67" priority="25" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="66" priority="22" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="66" priority="26" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="65" priority="23" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="65" priority="27" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="64" priority="24" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="64" priority="28" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H10))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="63" priority="25" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="63" priority="29" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H11))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="62" priority="26" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="62" priority="30" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H11))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="61" priority="27" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="61" priority="31" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H11))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="60" priority="28" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="60" priority="32" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H11))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="containsText" dxfId="59" priority="29" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="59" priority="33" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="containsText" dxfId="58" priority="30" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="58" priority="34" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="containsText" dxfId="57" priority="31" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="57" priority="35" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="containsText" dxfId="56" priority="32" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="56" priority="36" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="containsText" dxfId="55" priority="33" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="55" priority="37" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H13))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="containsText" dxfId="54" priority="34" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="54" priority="38" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H13))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="containsText" dxfId="53" priority="35" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="53" priority="39" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H13))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="containsText" dxfId="52" priority="36" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="52" priority="40" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H13))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="containsText" dxfId="51" priority="37" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="51" priority="41" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="containsText" dxfId="50" priority="38" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="50" priority="42" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="containsText" dxfId="49" priority="39" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="49" priority="43" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="containsText" dxfId="48" priority="40" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="48" priority="44" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="containsText" dxfId="47" priority="41" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H15))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="containsText" dxfId="46" priority="42" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H15))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="containsText" dxfId="45" priority="43" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="45" priority="47" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H15))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="containsText" dxfId="44" priority="44" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="44" priority="48" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H15))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="containsText" dxfId="43" priority="45" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="43" priority="49" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H16))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="containsText" dxfId="42" priority="46" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="42" priority="50" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H16))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="containsText" dxfId="41" priority="47" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="41" priority="51" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H16))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="containsText" dxfId="40" priority="48" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="40" priority="52" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H16))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="containsText" dxfId="39" priority="57" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="containsText" dxfId="38" priority="58" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="containsText" dxfId="37" priority="59" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="containsText" dxfId="36" priority="60" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="containsText" dxfId="35" priority="61" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="containsText" dxfId="34" priority="62" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="containsText" dxfId="33" priority="63" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="containsText" dxfId="32" priority="64" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="containsText" dxfId="31" priority="65" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="containsText" dxfId="30" priority="66" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="containsText" dxfId="29" priority="67" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="containsText" dxfId="28" priority="68" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="containsText" dxfId="27" priority="69" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="containsText" dxfId="26" priority="70" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="containsText" dxfId="25" priority="71" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="containsText" dxfId="24" priority="72" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="containsText" dxfId="23" priority="73" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="containsText" dxfId="22" priority="74" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="containsText" dxfId="21" priority="75" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="containsText" dxfId="20" priority="76" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="containsText" dxfId="19" priority="77" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="containsText" dxfId="18" priority="78" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="containsText" dxfId="17" priority="79" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="containsText" dxfId="16" priority="80" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="containsText" dxfId="15" priority="81" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="containsText" dxfId="14" priority="82" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="containsText" dxfId="13" priority="83" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="containsText" dxfId="12" priority="84" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25 H27:H28">
+    <cfRule type="containsText" dxfId="11" priority="85" operator="containsText" text="TO-DO">
+      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H25))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25 H27:H28">
+    <cfRule type="containsText" dxfId="10" priority="86" operator="containsText" text="DOING">
+      <formula>NOT(ISERROR(SEARCH(("DOING"),(H25))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25 H27:H28">
+    <cfRule type="containsText" dxfId="9" priority="87" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH(("DONE"),(H25))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25 H27:H28">
+    <cfRule type="containsText" dxfId="8" priority="88" operator="containsText" text="TO REWORK">
+      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H25))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="containsText" dxfId="39" priority="49" operator="containsText" text="TO-DO">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TO-DO">
       <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H17))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="containsText" dxfId="38" priority="50" operator="containsText" text="DOING">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="DOING">
       <formula>NOT(ISERROR(SEARCH(("DOING"),(H17))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="containsText" dxfId="37" priority="51" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH(("DONE"),(H17))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="containsText" dxfId="36" priority="52" operator="containsText" text="TO REWORK">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TO REWORK">
       <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H17))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
-    <cfRule type="containsText" dxfId="35" priority="53" operator="containsText" text="TO-DO">
-      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
-    <cfRule type="containsText" dxfId="34" priority="54" operator="containsText" text="DOING">
-      <formula>NOT(ISERROR(SEARCH(("DOING"),(H18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
-    <cfRule type="containsText" dxfId="33" priority="55" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH(("DONE"),(H18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
-    <cfRule type="containsText" dxfId="32" priority="56" operator="containsText" text="TO REWORK">
-      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
-    <cfRule type="containsText" dxfId="31" priority="57" operator="containsText" text="TO-DO">
-      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H19))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
-    <cfRule type="containsText" dxfId="30" priority="58" operator="containsText" text="DOING">
-      <formula>NOT(ISERROR(SEARCH(("DOING"),(H19))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
-    <cfRule type="containsText" dxfId="29" priority="59" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH(("DONE"),(H19))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
-    <cfRule type="containsText" dxfId="28" priority="60" operator="containsText" text="TO REWORK">
-      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H19))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
-    <cfRule type="containsText" dxfId="27" priority="61" operator="containsText" text="TO-DO">
-      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H20))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
-    <cfRule type="containsText" dxfId="26" priority="62" operator="containsText" text="DOING">
-      <formula>NOT(ISERROR(SEARCH(("DOING"),(H20))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
-    <cfRule type="containsText" dxfId="25" priority="63" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH(("DONE"),(H20))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
-    <cfRule type="containsText" dxfId="24" priority="64" operator="containsText" text="TO REWORK">
-      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H20))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="containsText" dxfId="23" priority="65" operator="containsText" text="TO-DO">
-      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H21))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="containsText" dxfId="22" priority="66" operator="containsText" text="DOING">
-      <formula>NOT(ISERROR(SEARCH(("DOING"),(H21))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="containsText" dxfId="21" priority="67" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH(("DONE"),(H21))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="containsText" dxfId="20" priority="68" operator="containsText" text="TO REWORK">
-      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H21))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
-    <cfRule type="containsText" dxfId="19" priority="69" operator="containsText" text="TO-DO">
-      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H22))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
-    <cfRule type="containsText" dxfId="18" priority="70" operator="containsText" text="DOING">
-      <formula>NOT(ISERROR(SEARCH(("DOING"),(H22))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
-    <cfRule type="containsText" dxfId="17" priority="71" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH(("DONE"),(H22))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
-    <cfRule type="containsText" dxfId="16" priority="72" operator="containsText" text="TO REWORK">
-      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H22))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
-    <cfRule type="containsText" dxfId="15" priority="73" operator="containsText" text="TO-DO">
-      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H23))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
-    <cfRule type="containsText" dxfId="14" priority="74" operator="containsText" text="DOING">
-      <formula>NOT(ISERROR(SEARCH(("DOING"),(H23))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
-    <cfRule type="containsText" dxfId="13" priority="75" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH(("DONE"),(H23))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
-    <cfRule type="containsText" dxfId="12" priority="76" operator="containsText" text="TO REWORK">
-      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H23))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="11" priority="77" operator="containsText" text="TO-DO">
-      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H24))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="10" priority="78" operator="containsText" text="DOING">
-      <formula>NOT(ISERROR(SEARCH(("DOING"),(H24))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="9" priority="79" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH(("DONE"),(H24))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
-    <cfRule type="containsText" dxfId="8" priority="80" operator="containsText" text="TO REWORK">
-      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H24))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25 H27:H28">
-    <cfRule type="containsText" dxfId="7" priority="81" operator="containsText" text="TO-DO">
-      <formula>NOT(ISERROR(SEARCH(("TO-DO"),(H25))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25 H27:H28">
-    <cfRule type="containsText" dxfId="6" priority="82" operator="containsText" text="DOING">
-      <formula>NOT(ISERROR(SEARCH(("DOING"),(H25))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25 H27:H28">
-    <cfRule type="containsText" dxfId="5" priority="83" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH(("DONE"),(H25))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25 H27:H28">
-    <cfRule type="containsText" dxfId="4" priority="84" operator="containsText" text="TO REWORK">
-      <formula>NOT(ISERROR(SEARCH(("TO REWORK"),(H25))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -30891,7 +31001,7 @@
           <x14:formula1>
             <xm:f>'()'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H4:H25 H27:H28</xm:sqref>
+          <xm:sqref>H27:H28 H4:H25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>